<commit_message>
Updates to Papers and Material Property Data Sheet
</commit_message>
<xml_diff>
--- a/Adhesive/Data.xlsx
+++ b/Adhesive/Data.xlsx
@@ -3,14 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10509"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90207C99-4787-D741-9CE1-7E9EE433B4E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C6FAAA1-9E90-7E4E-8180-F7D18C72B61B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="500" windowWidth="23200" windowHeight="15500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5520" yWindow="1040" windowWidth="28180" windowHeight="13800" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RawData" sheetId="1" r:id="rId1"/>
     <sheet name="Material" sheetId="2" r:id="rId2"/>
     <sheet name="Tests" sheetId="3" r:id="rId3"/>
+    <sheet name="Test1" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
@@ -30,8 +32,30 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="81">
   <si>
     <t>GT20</t>
   </si>
@@ -108,9 +132,6 @@
     <t>nu</t>
   </si>
   <si>
-    <t>Outer Point</t>
-  </si>
-  <si>
     <t>X Range</t>
   </si>
   <si>
@@ -120,34 +141,19 @@
     <t>Z Range</t>
   </si>
   <si>
-    <t>Differences</t>
-  </si>
-  <si>
     <t>R (mm)</t>
   </si>
   <si>
     <t>E min (Pa  = N/m^2)</t>
   </si>
   <si>
-    <t>E min (MPa  = N/mm^2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E max </t>
-  </si>
-  <si>
     <t>Steps</t>
-  </si>
-  <si>
-    <t>Difference</t>
   </si>
   <si>
     <t>Inner Points</t>
   </si>
   <si>
     <t>Outer Points</t>
-  </si>
-  <si>
-    <t>Aim</t>
   </si>
   <si>
     <t>Average</t>
@@ -159,10 +165,139 @@
     <t xml:space="preserve">Specific Step </t>
   </si>
   <si>
-    <t>Disp</t>
+    <t xml:space="preserve">mu </t>
   </si>
   <si>
-    <t>Specific Disp</t>
+    <t>Con/Div</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Form </t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>kappa</t>
+  </si>
+  <si>
+    <t>lambda</t>
+  </si>
+  <si>
+    <t>R+t</t>
+  </si>
+  <si>
+    <t>R+t after def</t>
+  </si>
+  <si>
+    <t>Applied Pressure</t>
+  </si>
+  <si>
+    <t>Specific pressure (Mpa)</t>
+  </si>
+  <si>
+    <t>MPa</t>
+  </si>
+  <si>
+    <t>Radius Max (mm)</t>
+  </si>
+  <si>
+    <t>Thickness</t>
+  </si>
+  <si>
+    <t>Thickness (mm)</t>
+  </si>
+  <si>
+    <t>E_p</t>
+  </si>
+  <si>
+    <t>E_s</t>
+  </si>
+  <si>
+    <t>nu_p</t>
+  </si>
+  <si>
+    <t>nu_s</t>
+  </si>
+  <si>
+    <t>mu_p</t>
+  </si>
+  <si>
+    <t>mu_s</t>
+  </si>
+  <si>
+    <t>res_r</t>
+  </si>
+  <si>
+    <t>res_rr</t>
+  </si>
+  <si>
+    <t>Max P</t>
+  </si>
+  <si>
+    <t>Div Pressure</t>
+  </si>
+  <si>
+    <t>Vertices</t>
+  </si>
+  <si>
+    <t>Cells</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shear and bulk were specified </t>
+  </si>
+  <si>
+    <t>E (Pa)</t>
+  </si>
+  <si>
+    <t>Div Step</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Initial Shear Mod (Pa)</t>
+  </si>
+  <si>
+    <t>Bulk Mod (Pa)</t>
+  </si>
+  <si>
+    <t>Min Shear Mod (Pa)</t>
+  </si>
+  <si>
+    <t>Max Shear Mod (Pa)</t>
+  </si>
+  <si>
+    <t>E min (Pa)</t>
+  </si>
+  <si>
+    <t>Wall thickness</t>
+  </si>
+  <si>
+    <t>Glandular</t>
+  </si>
+  <si>
+    <t>Forestomach</t>
+  </si>
+  <si>
+    <t>0.9+-0.1</t>
+  </si>
+  <si>
+    <t>0.5+-0.1</t>
+  </si>
+  <si>
+    <t>Zhao (Rat Model)</t>
+  </si>
+  <si>
+    <t>Saraf (Human)</t>
+  </si>
+  <si>
+    <t>Skamniotis (Human</t>
+  </si>
+  <si>
+    <t>FINAL</t>
   </si>
 </sst>
 </file>
@@ -197,7 +332,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -207,6 +342,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -223,7 +364,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -237,6 +378,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -11245,16 +11393,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>165100</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>88900</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>25400</xdr:colOff>
+      <xdr:colOff>622300</xdr:colOff>
       <xdr:row>21</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -11548,7 +11696,7 @@
   <dimension ref="A1:M3306"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -77024,59 +77172,56 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E532B5D-9B22-CE40-B35C-CCABE218B090}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
     <col min="2" max="2" width="12.33203125" customWidth="1"/>
-    <col min="4" max="4" width="11.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="F1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
-        <v>32</v>
-      </c>
-      <c r="I1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="10">
         <v>0.47499999999999998</v>
       </c>
       <c r="C2">
-        <v>480000</v>
-      </c>
-      <c r="D2">
+        <v>480000000</v>
+      </c>
+      <c r="D2" s="10">
         <v>8000</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="10">
         <v>45000</v>
       </c>
       <c r="F2">
@@ -77087,20 +77232,12 @@
         <f>2*E2*(1+B2)</f>
         <v>132750</v>
       </c>
-      <c r="H2">
-        <f>F2/(1000^2)</f>
-        <v>2.3599999999999999E-2</v>
-      </c>
-      <c r="I2">
-        <f>G2/(1000^2)</f>
-        <v>0.13275000000000001</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="10">
         <v>0.49</v>
       </c>
       <c r="C3">
@@ -77111,160 +77248,430 @@
         <f>G3/(2*(1+B3))</f>
         <v>36.818791946308721</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="10">
         <v>109.72</v>
       </c>
-      <c r="I3">
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>C2/(1000^2)</f>
+        <v>480</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="C5:E6" si="0">D2/(1000^2)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F5">
+        <f>F2/(1000^2)</f>
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="G5">
+        <f>G2/(1000^2)</f>
+        <v>0.13275000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1.8286666666666649E-3</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>3.6818791946308721E-5</v>
+      </c>
+      <c r="G6">
         <f>G3/(1000^2)</f>
         <v>1.0972E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G8" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C9" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D9" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E9" t="s">
         <v>19</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G9" t="s">
         <v>18</v>
       </c>
-      <c r="H6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="H9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B7">
+      <c r="B10">
         <v>1.5</v>
       </c>
-      <c r="C7">
+      <c r="C10">
         <v>2</v>
       </c>
-      <c r="D7">
-        <f>POWER(B7*3/(4*PI()),1/3)</f>
+      <c r="D10">
+        <f>POWER(B10*3/(4*PI()),1/3)</f>
         <v>0.71012404230749426</v>
       </c>
-      <c r="E7">
-        <f>POWER(C7*3/(4*PI()),1/3)</f>
+      <c r="E10">
+        <f>POWER(C10*3/(4*PI()),1/3)</f>
         <v>0.78159264179677201</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B8">
-        <f>B7+0.9</f>
+      <c r="B11">
+        <f>B10+0.9</f>
         <v>2.4</v>
       </c>
-      <c r="C8">
-        <f>C7+0.9</f>
+      <c r="C11">
+        <f>C10+0.9</f>
         <v>2.9</v>
       </c>
-      <c r="D8">
-        <f>POWER(B8*3/(4*PI()),1/3)</f>
+      <c r="D11">
+        <f>POWER(B11*3/(4*PI()),1/3)</f>
         <v>0.83056611841541483</v>
       </c>
-      <c r="E8">
-        <f>POWER(C8*3/(4*PI()),1/3)</f>
+      <c r="E11">
+        <f>POWER(C11*3/(4*PI()),1/3)</f>
         <v>0.88464656637351857</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D9" t="s">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D12" t="s">
         <v>20</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E12" t="s">
         <v>20</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G12" t="s">
         <v>20</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D10">
-        <f>D7*10</f>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13">
+        <v>0.5</v>
+      </c>
+      <c r="D13" s="6">
+        <f>D10*10</f>
         <v>7.1012404230749429</v>
       </c>
-      <c r="E10">
-        <f>E7*10</f>
+      <c r="E13">
+        <f>E10*10</f>
         <v>7.8159264179677201</v>
       </c>
-      <c r="G10">
-        <f t="shared" ref="G10:H12" si="0">D10+0.5</f>
+      <c r="G13" s="6">
+        <f>D13+$B$13</f>
         <v>7.6012404230749429</v>
       </c>
-      <c r="H10">
-        <f t="shared" si="0"/>
+      <c r="H13" s="9">
+        <f>E13+$B$13</f>
         <v>8.3159264179677201</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D11">
-        <f>D8*10</f>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="D14" s="6">
+        <f>D11*10</f>
         <v>8.3056611841541486</v>
       </c>
-      <c r="E11">
-        <f>E8*10</f>
+      <c r="E14">
+        <f>E11*10</f>
         <v>8.8464656637351862</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="0"/>
+      <c r="G14" s="6">
+        <f>D14+$B$13</f>
         <v>8.8056611841541486</v>
       </c>
-      <c r="H11">
-        <f t="shared" si="0"/>
+      <c r="H14" s="9">
+        <f>E14+$B$13</f>
         <v>9.3464656637351862</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12">
-        <f>D11-D10</f>
-        <v>1.2044207610792057</v>
-      </c>
-      <c r="E12">
-        <f>E11-E10</f>
-        <v>1.030539245767466</v>
-      </c>
-      <c r="F12" t="s">
-        <v>35</v>
-      </c>
-      <c r="G12">
-        <f t="shared" si="0"/>
-        <v>1.7044207610792057</v>
-      </c>
-      <c r="H12">
-        <f t="shared" si="0"/>
-        <v>1.530539245767466</v>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17">
+        <f>(3*(C17/D17)-2)/(6*C17/D17+2)</f>
+        <v>0.47540983606557374</v>
+      </c>
+      <c r="C17">
+        <f>2000*1000</f>
+        <v>2000000</v>
+      </c>
+      <c r="D17">
+        <f>100*1000</f>
+        <v>100000</v>
+      </c>
+      <c r="E17">
+        <f>2*D17*(1+B17)</f>
+        <v>295081.96721311472</v>
+      </c>
+      <c r="F17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <f>C17/1000^2</f>
+        <v>2</v>
+      </c>
+      <c r="D19" s="10">
+        <f>D17/1000^2</f>
+        <v>0.1</v>
+      </c>
+      <c r="E19">
+        <f>E17/1000^2</f>
+        <v>0.29508196721311475</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B20" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G20" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>78</v>
+      </c>
+      <c r="B21">
+        <v>0.47540983606557374</v>
+      </c>
+      <c r="C21">
+        <f>0.48*10^9</f>
+        <v>480000000</v>
+      </c>
+      <c r="D21">
+        <f>8*1000</f>
+        <v>8000</v>
+      </c>
+      <c r="E21">
+        <f>45*1000</f>
+        <v>45000</v>
+      </c>
+      <c r="F21">
+        <f>2*D21*(1+B21)</f>
+        <v>23606.557377049179</v>
+      </c>
+      <c r="G21">
+        <f>2*E21*(1+B21)</f>
+        <v>132786.88524590162</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C22" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" t="s">
+        <v>46</v>
+      </c>
+      <c r="G22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <f>C21/(1000^2)</f>
+        <v>480</v>
+      </c>
+      <c r="D23" s="10">
+        <f t="shared" ref="D23:G23" si="1">D21/(1000^2)</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E23" s="10">
+        <f t="shared" si="1"/>
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="1"/>
+        <v>2.360655737704918E-2</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>0.13278688524590163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J24" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>77</v>
+      </c>
+      <c r="B25">
+        <v>0.45</v>
+      </c>
+      <c r="D25">
+        <f>E25/(2*(1+B25))</f>
+        <v>28620.689655172413</v>
+      </c>
+      <c r="E25">
+        <f>83*1000</f>
+        <v>83000</v>
+      </c>
+      <c r="H25" t="s">
+        <v>20</v>
+      </c>
+      <c r="I25" t="s">
+        <v>75</v>
+      </c>
+      <c r="J25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <f>C25/1000^2</f>
+        <v>0</v>
+      </c>
+      <c r="D27" s="10">
+        <f>D25/1000^2</f>
+        <v>2.8620689655172414E-2</v>
+      </c>
+      <c r="E27">
+        <f>E25/1000^2</f>
+        <v>8.3000000000000004E-2</v>
       </c>
     </row>
   </sheetData>
@@ -77274,51 +77681,41 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE7B6CA-A3F6-0748-BC26-30E6FFC6A2B7}">
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:Z22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="4" customWidth="1"/>
+    <col min="1" max="2" width="4.6640625" customWidth="1"/>
+    <col min="3" max="3" width="5.5" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="5" max="5" width="5.83203125" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" customWidth="1"/>
-    <col min="9" max="9" width="7.5" customWidth="1"/>
-    <col min="10" max="10" width="7.6640625" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" customWidth="1"/>
-    <col min="12" max="12" width="7.1640625" customWidth="1"/>
-    <col min="13" max="13" width="7.5" customWidth="1"/>
-    <col min="14" max="14" width="6" customWidth="1"/>
-    <col min="15" max="15" width="7" customWidth="1"/>
-    <col min="16" max="16" width="8.33203125" customWidth="1"/>
-    <col min="17" max="17" width="8.1640625" customWidth="1"/>
+    <col min="5" max="8" width="5.83203125" customWidth="1"/>
+    <col min="9" max="9" width="4" customWidth="1"/>
+    <col min="10" max="10" width="6.5" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
+    <col min="13" max="13" width="8.5" customWidth="1"/>
+    <col min="14" max="14" width="8.1640625" customWidth="1"/>
+    <col min="15" max="15" width="7.5" customWidth="1"/>
+    <col min="16" max="16" width="7.6640625" customWidth="1"/>
+    <col min="17" max="17" width="8.6640625" customWidth="1"/>
     <col min="18" max="18" width="7.1640625" customWidth="1"/>
     <col min="19" max="19" width="7.5" customWidth="1"/>
-    <col min="20" max="20" width="8.33203125" customWidth="1"/>
-    <col min="21" max="21" width="5" customWidth="1"/>
+    <col min="20" max="20" width="7.6640625" customWidth="1"/>
+    <col min="21" max="21" width="8.83203125" customWidth="1"/>
     <col min="22" max="22" width="9.5" customWidth="1"/>
     <col min="23" max="23" width="4.6640625" customWidth="1"/>
     <col min="24" max="24" width="5.33203125" customWidth="1"/>
     <col min="25" max="25" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C1" t="s">
-        <v>22</v>
-      </c>
       <c r="D1" t="s">
         <v>23</v>
       </c>
@@ -77326,56 +77723,66 @@
         <v>24</v>
       </c>
       <c r="F1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="N1" s="7"/>
+      <c r="O1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5" t="s">
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="L1" s="5"/>
-      <c r="M1" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
-      <c r="P1" s="5"/>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="3" t="s">
+      <c r="R1" s="7"/>
+      <c r="S1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="T1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W1" t="s">
+        <v>44</v>
+      </c>
+      <c r="X1" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="Z1" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="W1" t="s">
-        <v>42</v>
-      </c>
-      <c r="X1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0.8</v>
-      </c>
-      <c r="B2">
-        <v>7.1012000000000004</v>
-      </c>
-      <c r="C2">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="D2">
         <v>2.3599999999999999E-2</v>
@@ -77384,262 +77791,272 @@
         <v>0.47499999999999998</v>
       </c>
       <c r="F2">
-        <f>B2+C2</f>
+        <f>D2/(2*(1+E2))</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G2">
+        <f>D2*E2/((1+E2)*(1-2*E2))</f>
+        <v>0.15199999999999986</v>
+      </c>
+      <c r="H2">
+        <f>G2+2*F2/3</f>
+        <v>0.15733333333333319</v>
+      </c>
+      <c r="I2">
+        <v>0.5</v>
+      </c>
+      <c r="J2">
+        <v>7.1012000000000004</v>
+      </c>
+      <c r="K2">
+        <f>J2+I2</f>
         <v>7.6012000000000004</v>
       </c>
-      <c r="G2">
-        <v>-9.1419200000000007</v>
-      </c>
-      <c r="H2">
-        <v>9.0982000000000003</v>
-      </c>
-      <c r="I2">
-        <v>-9.1229600000000008</v>
-      </c>
-      <c r="J2">
-        <v>9.1220599999999994</v>
-      </c>
-      <c r="K2">
-        <v>-9.1400299999999994</v>
-      </c>
       <c r="L2">
-        <v>9.1034000000000006</v>
+        <v>8.8056611839999999</v>
       </c>
       <c r="M2">
-        <f t="shared" ref="M2:R2" si="0">ABS(G2)-$F$2</f>
-        <v>1.5407200000000003</v>
+        <v>-8.3254199999999994</v>
       </c>
       <c r="N2">
-        <f t="shared" si="0"/>
-        <v>1.4969999999999999</v>
+        <v>8.3015000000000008</v>
       </c>
       <c r="O2">
-        <f t="shared" si="0"/>
-        <v>1.5217600000000004</v>
+        <v>-8.3088200000000008</v>
       </c>
       <c r="P2">
-        <f t="shared" si="0"/>
-        <v>1.520859999999999</v>
+        <v>8.2932299999999994</v>
       </c>
       <c r="Q2">
-        <f t="shared" si="0"/>
-        <v>1.538829999999999</v>
+        <v>-8.3231599999999997</v>
       </c>
       <c r="R2">
-        <f t="shared" si="0"/>
-        <v>1.5022000000000002</v>
-      </c>
-      <c r="S2">
-        <f>AVERAGE(M2:R2)</f>
-        <v>1.5202283333333331</v>
+        <v>8.3013899999999996</v>
+      </c>
+      <c r="S2" cm="1">
+        <f t="array" ref="S2">AVERAGE(ABS(M2:R2))</f>
+        <v>8.3089199999999988</v>
       </c>
       <c r="T2">
-        <v>1.704420761</v>
-      </c>
-      <c r="U2">
-        <v>12</v>
-      </c>
-      <c r="V2">
-        <v>1.21212E-2</v>
-      </c>
+        <f>ABS(L2-S2)/L2*100</f>
+        <v>5.6411571331246115</v>
+      </c>
+      <c r="U2" s="4">
+        <v>22</v>
+      </c>
+      <c r="V2" s="4"/>
       <c r="W2">
         <v>0.1</v>
       </c>
       <c r="X2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="L3">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M3">
+        <v>-8.6249300000000009</v>
+      </c>
+      <c r="N3">
+        <v>8.5906800000000008</v>
+      </c>
+      <c r="O3">
+        <v>-8.5812399999999993</v>
+      </c>
+      <c r="P3">
+        <v>8.5621799999999997</v>
+      </c>
+      <c r="Q3">
+        <v>-8.6197999999999997</v>
+      </c>
+      <c r="R3">
+        <v>8.5925499999999992</v>
+      </c>
+      <c r="S3" cm="1">
+        <f t="array" ref="S3">AVERAGE(ABS(M3:R3))</f>
+        <v>8.595229999999999</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T20" si="0">ABS(L3-S3)/L3*100</f>
+        <v>2.3897261046377416</v>
+      </c>
+      <c r="U3">
+        <v>29</v>
+      </c>
+      <c r="X3">
         <v>100</v>
       </c>
-      <c r="Y2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="G3">
-        <v>-9.1292000000000009</v>
-      </c>
-      <c r="H3">
-        <v>9.0859500000000004</v>
-      </c>
-      <c r="I3">
-        <v>-9.1098700000000008</v>
-      </c>
-      <c r="J3">
-        <v>9.1092700000000004</v>
-      </c>
-      <c r="K3">
-        <v>-9.1271100000000001</v>
-      </c>
-      <c r="L3">
-        <v>9.0899800000000006</v>
-      </c>
-      <c r="M3">
-        <f>ABS(G3)-$F$2</f>
-        <v>1.5280000000000005</v>
-      </c>
-      <c r="N3">
-        <f t="shared" ref="N3:R3" si="1">ABS(H3)-$F$2</f>
-        <v>1.48475</v>
-      </c>
-      <c r="O3">
-        <f t="shared" si="1"/>
-        <v>1.5086700000000004</v>
-      </c>
-      <c r="P3">
-        <f t="shared" si="1"/>
-        <v>1.50807</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" si="1"/>
-        <v>1.5259099999999997</v>
-      </c>
-      <c r="R3">
-        <f t="shared" si="1"/>
-        <v>1.4887800000000002</v>
-      </c>
-      <c r="S3">
-        <f>AVERAGE(M3:R3)</f>
-        <v>1.5073633333333334</v>
-      </c>
-      <c r="T3">
-        <v>1.704420761</v>
-      </c>
-      <c r="U3">
-        <v>24</v>
-      </c>
-      <c r="V3">
-        <v>1.2060299999999999E-2</v>
-      </c>
-      <c r="W3">
+      <c r="Y3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>0.6</v>
+      </c>
+      <c r="D4">
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="E4">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F4">
+        <f>D4/(2*(1+E4))</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G19" si="1">D4*E4/((1+E4)*(1-2*E4))</f>
+        <v>0.15199999999999986</v>
+      </c>
+      <c r="H4">
+        <f>G4+2*F4/3</f>
+        <v>0.15733333333333319</v>
+      </c>
+      <c r="I4">
+        <v>0.5</v>
+      </c>
+      <c r="J4">
+        <v>7.1012000000000004</v>
+      </c>
+      <c r="K4">
+        <f>J4+I4</f>
+        <v>7.6012000000000004</v>
+      </c>
+      <c r="U4">
+        <v>32</v>
+      </c>
+      <c r="V4">
+        <v>1.5075369999999999E-2</v>
+      </c>
+      <c r="X4">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="L5">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M5">
+        <v>-8.6938899999999997</v>
+      </c>
+      <c r="N5">
+        <v>8.6767800000000008</v>
+      </c>
+      <c r="O5">
+        <v>-8.6787600000000005</v>
+      </c>
+      <c r="P5">
+        <v>8.6516500000000001</v>
+      </c>
+      <c r="Q5">
+        <v>-8.7293900000000004</v>
+      </c>
+      <c r="R5">
+        <v>8.6826899999999991</v>
+      </c>
+      <c r="S5" cm="1">
+        <f t="array" ref="S5">AVERAGE(ABS(M5:R5))</f>
+        <v>8.6855266666666679</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>1.3642873013512931</v>
+      </c>
+      <c r="U5">
+        <v>62</v>
+      </c>
+      <c r="V5">
+        <v>1.5538847117700001E-2</v>
+      </c>
+      <c r="X5">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="L6">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M6">
+        <v>-8.7072599999999998</v>
+      </c>
+      <c r="N6">
+        <v>8.6921499999999998</v>
+      </c>
+      <c r="O6">
+        <v>-8.6939299999999999</v>
+      </c>
+      <c r="P6">
+        <v>8.6645500000000002</v>
+      </c>
+      <c r="Q6">
+        <v>-8.7439300000000006</v>
+      </c>
+      <c r="R6">
+        <v>8.6996699999999993</v>
+      </c>
+      <c r="S6" cm="1">
+        <f t="array" ref="S6">AVERAGE(ABS(M6:R6))</f>
+        <v>8.7002483333333327</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>1.1971031869611755</v>
+      </c>
+      <c r="U6">
+        <v>95</v>
+      </c>
+      <c r="V6">
+        <v>1.5689999999999999E-2</v>
+      </c>
+      <c r="X6">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="L7">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M7">
+        <v>-8.6917600000000004</v>
+      </c>
+      <c r="N7">
+        <v>8.6745800000000006</v>
+      </c>
+      <c r="O7">
+        <v>-8.6766000000000005</v>
+      </c>
+      <c r="P7">
+        <v>8.6495800000000003</v>
+      </c>
+      <c r="Q7">
+        <v>-8.7271599999999996</v>
+      </c>
+      <c r="R7">
+        <v>8.6804900000000007</v>
+      </c>
+      <c r="S7" cm="1">
+        <f t="array" ref="S7">AVERAGE(ABS(M7:R7))</f>
+        <v>8.6833616666666664</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>1.388873757209206</v>
+      </c>
+      <c r="V7">
+        <v>1.55155E-2</v>
+      </c>
+      <c r="W7">
         <v>0.1</v>
       </c>
-      <c r="X3">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="W4">
-        <v>0.1</v>
-      </c>
-      <c r="X4">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="W5">
-        <v>0.1</v>
-      </c>
-      <c r="X5">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="G6">
-        <v>-9.2023899999999994</v>
-      </c>
-      <c r="H6">
-        <v>9.1579700000000006</v>
-      </c>
-      <c r="I6">
-        <v>-9.1853300000000004</v>
-      </c>
-      <c r="J6">
-        <v>9.1822199999999992</v>
-      </c>
-      <c r="K6">
-        <v>-9.2028800000000004</v>
-      </c>
-      <c r="L6">
-        <v>9.16892</v>
-      </c>
-      <c r="M6">
-        <f>ABS(G6)-$F$2</f>
-        <v>1.601189999999999</v>
-      </c>
-      <c r="N6">
-        <f t="shared" ref="N6:R6" si="2">ABS(H6)-$F$2</f>
-        <v>1.5567700000000002</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="2"/>
-        <v>1.58413</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="2"/>
-        <v>1.5810199999999988</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="2"/>
-        <v>1.60168</v>
-      </c>
-      <c r="R6">
-        <f t="shared" si="2"/>
-        <v>1.5677199999999996</v>
-      </c>
-      <c r="S6">
-        <f>AVERAGE(M6:R6)</f>
-        <v>1.5820849999999995</v>
-      </c>
-      <c r="T6">
-        <v>1.704420761</v>
-      </c>
-      <c r="U6">
-        <v>124</v>
-      </c>
-      <c r="X6">
+      <c r="X7">
         <v>1000</v>
       </c>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A7" s="6">
-        <v>0.4</v>
-      </c>
-      <c r="B7" s="6">
-        <v>7.1012000000000004</v>
-      </c>
-      <c r="C7" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="D7" s="6">
-        <v>2.3599999999999999E-2</v>
-      </c>
-      <c r="E7" s="6">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="F7" s="6">
-        <f>B7+C7</f>
-        <v>7.6012000000000004</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
-      <c r="U7" s="6"/>
-      <c r="V7" s="6"/>
-      <c r="W7" s="6">
-        <v>0.1</v>
-      </c>
-      <c r="X7" s="6">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>0.4</v>
-      </c>
-      <c r="B9">
-        <v>7.1012000000000004</v>
-      </c>
-      <c r="C9">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="D9">
         <v>2.3599999999999999E-2</v>
@@ -77648,346 +78065,1267 @@
         <v>0.47499999999999998</v>
       </c>
       <c r="F9">
-        <f>B9+C9</f>
+        <f>D9/(2*(1+E9))</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>0.15199999999999986</v>
+      </c>
+      <c r="H9">
+        <f>G9+2*F9/3</f>
+        <v>0.15733333333333319</v>
+      </c>
+      <c r="I9">
+        <v>0.5</v>
+      </c>
+      <c r="J9">
+        <v>7.1012000000000004</v>
+      </c>
+      <c r="K9">
+        <f>J9+I9</f>
         <v>7.6012000000000004</v>
       </c>
-      <c r="G9">
-        <v>-8.3254199999999994</v>
-      </c>
-      <c r="H9">
-        <v>8.3015000000000008</v>
-      </c>
-      <c r="I9">
-        <v>-8.3088200000000008</v>
-      </c>
-      <c r="J9">
-        <v>8.2932299999999994</v>
-      </c>
-      <c r="K9">
-        <v>8.3231599999999997</v>
-      </c>
       <c r="L9">
-        <v>8.3013899999999996</v>
+        <v>8.8056611839999999</v>
       </c>
       <c r="M9">
-        <f t="shared" ref="M9:M10" si="3">ABS(G9)-$F$2</f>
-        <v>0.72421999999999898</v>
+        <v>-9.1419200000000007</v>
       </c>
       <c r="N9">
-        <f t="shared" ref="N9:N10" si="4">ABS(H9)-$F$2</f>
-        <v>0.70030000000000037</v>
+        <v>9.0982000000000003</v>
       </c>
       <c r="O9">
-        <f t="shared" ref="O9:O10" si="5">ABS(I9)-$F$2</f>
-        <v>0.70762000000000036</v>
+        <v>-9.1229600000000008</v>
       </c>
       <c r="P9">
-        <f t="shared" ref="P9:P10" si="6">ABS(J9)-$F$2</f>
-        <v>0.69202999999999903</v>
+        <v>9.1220599999999994</v>
       </c>
       <c r="Q9">
-        <f t="shared" ref="Q9:Q10" si="7">ABS(K9)-$F$2</f>
-        <v>0.72195999999999927</v>
+        <v>-9.1400299999999994</v>
       </c>
       <c r="R9">
-        <f t="shared" ref="R9:R10" si="8">ABS(L9)-$F$2</f>
-        <v>0.7001899999999992</v>
-      </c>
-      <c r="S9">
-        <f t="shared" ref="S9:S10" si="9">AVERAGE(M9:R9)</f>
-        <v>0.70771999999999957</v>
-      </c>
-      <c r="T9" s="4">
-        <v>1.7044207600000001</v>
-      </c>
-      <c r="U9" s="4">
-        <v>22</v>
-      </c>
-      <c r="V9" s="4"/>
+        <v>9.1034000000000006</v>
+      </c>
+      <c r="S9" cm="1">
+        <f t="array" ref="S9">AVERAGE(ABS(M9:R9))</f>
+        <v>9.1214283333333324</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>3.5859561563314006</v>
+      </c>
+      <c r="U9">
+        <v>12</v>
+      </c>
+      <c r="V9">
+        <v>1.21212E-2</v>
+      </c>
       <c r="W9">
         <v>0.1</v>
       </c>
-      <c r="X9">
+      <c r="X9" s="9">
+        <v>100</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="L10">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M10">
+        <v>-9.1292000000000009</v>
+      </c>
+      <c r="N10">
+        <v>9.0859500000000004</v>
+      </c>
+      <c r="O10">
+        <v>-9.1098700000000008</v>
+      </c>
+      <c r="P10">
+        <v>9.1092700000000004</v>
+      </c>
+      <c r="Q10">
+        <v>-9.1271100000000001</v>
+      </c>
+      <c r="R10">
+        <v>9.0899800000000006</v>
+      </c>
+      <c r="S10" cm="1">
+        <f t="array" ref="S10">AVERAGE(ABS(M10:R10))</f>
+        <v>9.1085633333333345</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>3.4398569625153383</v>
+      </c>
+      <c r="U10">
+        <v>24</v>
+      </c>
+      <c r="V10">
+        <v>1.2060299999999999E-2</v>
+      </c>
+      <c r="W10">
+        <v>0.1</v>
+      </c>
+      <c r="X10" s="9">
         <v>200</v>
       </c>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="G10">
-        <v>-8.6249300000000009</v>
-      </c>
-      <c r="H10">
-        <v>8.5906800000000008</v>
-      </c>
-      <c r="I10">
-        <v>-8.5812399999999993</v>
-      </c>
-      <c r="J10">
-        <v>8.5621799999999997</v>
-      </c>
-      <c r="K10">
-        <v>-8.6197999999999997</v>
-      </c>
-      <c r="L10">
-        <v>8.5925499999999992</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="3"/>
-        <v>1.0237300000000005</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="4"/>
-        <v>0.98948000000000036</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="5"/>
-        <v>0.98003999999999891</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="6"/>
-        <v>0.96097999999999928</v>
-      </c>
-      <c r="Q10">
-        <f t="shared" si="7"/>
-        <v>1.0185999999999993</v>
-      </c>
-      <c r="R10">
-        <f t="shared" si="8"/>
-        <v>0.99134999999999884</v>
-      </c>
-      <c r="S10">
-        <f t="shared" si="9"/>
-        <v>0.99402999999999953</v>
-      </c>
-      <c r="T10" s="4">
-        <v>1.7044207600000001</v>
-      </c>
-      <c r="U10">
-        <v>29</v>
-      </c>
-      <c r="X10">
-        <v>100</v>
-      </c>
-      <c r="Y10" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>0.6</v>
-      </c>
-      <c r="B11">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="L11">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M11">
+        <v>-9.2275200000000002</v>
+      </c>
+      <c r="N11">
+        <v>9.1812199999999997</v>
+      </c>
+      <c r="O11">
+        <v>-9.2101500000000005</v>
+      </c>
+      <c r="P11">
+        <v>9.2059499999999996</v>
+      </c>
+      <c r="Q11">
+        <v>-9.2312700000000003</v>
+      </c>
+      <c r="R11">
+        <v>9.1965199999999996</v>
+      </c>
+      <c r="S11" cm="1">
+        <f t="array" ref="S11">AVERAGE(ABS(M11:R11))</f>
+        <v>9.2087716666666672</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>4.5778559297639605</v>
+      </c>
+      <c r="U11">
+        <v>53</v>
+      </c>
+      <c r="V11">
+        <v>1.32832E-2</v>
+      </c>
+      <c r="W11">
+        <v>0.1</v>
+      </c>
+      <c r="X11" s="9">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="L12">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M12">
+        <v>-9.2253000000000007</v>
+      </c>
+      <c r="N12">
+        <v>9.1792700000000007</v>
+      </c>
+      <c r="O12">
+        <v>-9.2079799999999992</v>
+      </c>
+      <c r="P12">
+        <v>9.2038600000000006</v>
+      </c>
+      <c r="Q12">
+        <v>-9.22879</v>
+      </c>
+      <c r="R12">
+        <v>9.1940600000000003</v>
+      </c>
+      <c r="S12" cm="1">
+        <f t="array" ref="S12">AVERAGE(ABS(M12:R12))</f>
+        <v>9.2065433333333324</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>4.5525502396315298</v>
+      </c>
+      <c r="U12">
+        <v>77</v>
+      </c>
+      <c r="V12">
+        <v>1.28548E-2</v>
+      </c>
+      <c r="W12">
+        <v>0.1</v>
+      </c>
+      <c r="X12" s="9">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="L13">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M13">
+        <v>-9.2445400000000006</v>
+      </c>
+      <c r="N13">
+        <v>9.1967999999999996</v>
+      </c>
+      <c r="O13">
+        <v>-9.2269500000000004</v>
+      </c>
+      <c r="P13">
+        <v>9.2221700000000002</v>
+      </c>
+      <c r="Q13">
+        <v>-9.2481299999999997</v>
+      </c>
+      <c r="R13">
+        <v>9.2154000000000007</v>
+      </c>
+      <c r="S13" cm="1">
+        <f t="array" ref="S13">AVERAGE(ABS(M13:R13))</f>
+        <v>9.2256649999999993</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="0"/>
+        <v>4.7697022088829835</v>
+      </c>
+      <c r="U13">
+        <v>143</v>
+      </c>
+      <c r="V13">
+        <v>1.43143E-2</v>
+      </c>
+      <c r="W13">
+        <v>0.1</v>
+      </c>
+      <c r="X13" s="9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="L14">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M14">
+        <v>-8.8888200000000008</v>
+      </c>
+      <c r="N14">
+        <v>8.8558599999999998</v>
+      </c>
+      <c r="O14">
+        <v>-8.8668899999999997</v>
+      </c>
+      <c r="P14">
+        <v>8.8668099999999992</v>
+      </c>
+      <c r="Q14">
+        <v>-8.8873899999999999</v>
+      </c>
+      <c r="R14">
+        <v>8.8472899999999992</v>
+      </c>
+      <c r="S14" cm="1">
+        <f t="array" ref="S14">AVERAGE(ABS(M14:R14))</f>
+        <v>8.8688433333333325</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="0"/>
+        <v>0.71751737902584123</v>
+      </c>
+      <c r="U14">
+        <v>109</v>
+      </c>
+      <c r="V14">
+        <v>1.0910899999999999E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="L15">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M15">
+        <v>-8.8681900000000002</v>
+      </c>
+      <c r="N15">
+        <v>8.8359100000000002</v>
+      </c>
+      <c r="O15">
+        <v>-8.8463600000000007</v>
+      </c>
+      <c r="P15">
+        <v>8.8461400000000001</v>
+      </c>
+      <c r="Q15">
+        <v>-8.8669399999999996</v>
+      </c>
+      <c r="R15">
+        <v>8.8269800000000007</v>
+      </c>
+      <c r="S15" cm="1">
+        <f t="array" ref="S15">AVERAGE(ABS(N15:R15))</f>
+        <v>8.8444660000000006</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="0"/>
+        <v>0.44068032131998891</v>
+      </c>
+      <c r="U15">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="L16">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M16">
+        <v>-8.8476599999999994</v>
+      </c>
+      <c r="N16">
+        <v>8.8160399999999992</v>
+      </c>
+      <c r="O16">
+        <v>-8.8259699999999999</v>
+      </c>
+      <c r="P16">
+        <v>8.8255800000000004</v>
+      </c>
+      <c r="Q16">
+        <v>-8.8466000000000005</v>
+      </c>
+      <c r="R16">
+        <v>8.8068200000000001</v>
+      </c>
+      <c r="S16" cm="1">
+        <f t="array" ref="S16">AVERAGE(ABS(N16:R16))</f>
+        <v>8.8242020000000014</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="0"/>
+        <v>0.21055563702235638</v>
+      </c>
+      <c r="U16">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="L17" s="10">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M17" s="10">
+        <v>-8.8272499999999994</v>
+      </c>
+      <c r="N17" s="10">
+        <v>8.7962600000000002</v>
+      </c>
+      <c r="O17" s="10">
+        <v>-8.8057200000000009</v>
+      </c>
+      <c r="P17" s="10">
+        <v>8.80518</v>
+      </c>
+      <c r="Q17" s="10">
+        <v>-8.8263599999999993</v>
+      </c>
+      <c r="R17" s="10">
+        <v>8.7868099999999991</v>
+      </c>
+      <c r="S17" s="10" cm="1">
+        <f t="array" ref="S17">AVERAGE(ABS(N17:R17))</f>
+        <v>8.8040660000000006</v>
+      </c>
+      <c r="T17" s="10">
+        <f t="shared" si="0"/>
+        <v>1.8115436952056706E-2</v>
+      </c>
+      <c r="U17" s="10">
+        <v>106</v>
+      </c>
+      <c r="V17" s="10">
+        <v>1.06106E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:24" s="9" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
+        <v>0.4</v>
+      </c>
+      <c r="D19" s="9">
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="F19" s="9">
+        <f>D19/(2*(1+E19))</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G19" s="9">
+        <f t="shared" si="1"/>
+        <v>0.15199999999999986</v>
+      </c>
+      <c r="H19" s="9">
+        <f>G19+2*F19/3</f>
+        <v>0.15733333333333319</v>
+      </c>
+      <c r="I19" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="J19" s="9">
         <v>7.1012000000000004</v>
       </c>
-      <c r="C11">
-        <v>0.5</v>
-      </c>
-      <c r="D11">
-        <v>2.3599999999999999E-2</v>
-      </c>
-      <c r="E11">
-        <v>0.47499999999999998</v>
-      </c>
-      <c r="F11">
-        <f>B11+C11</f>
+      <c r="K19" s="9">
+        <f>J19+I19</f>
         <v>7.6012000000000004</v>
       </c>
-      <c r="U11">
-        <v>32</v>
-      </c>
-      <c r="V11">
-        <v>1.5075369999999999E-2</v>
-      </c>
-      <c r="X11">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="G12">
-        <v>-8.6938899999999997</v>
-      </c>
-      <c r="H12">
-        <v>8.6767800000000008</v>
-      </c>
-      <c r="I12">
-        <v>-8.6787600000000005</v>
-      </c>
-      <c r="J12">
-        <v>8.6516500000000001</v>
-      </c>
-      <c r="K12">
-        <v>-8.7293900000000004</v>
-      </c>
-      <c r="L12">
-        <v>8.6826899999999991</v>
-      </c>
-      <c r="M12">
-        <f>ABS(G12)-$F$2</f>
-        <v>1.0926899999999993</v>
-      </c>
-      <c r="N12">
-        <f t="shared" ref="N12:R14" si="10">ABS(H12)-$F$2</f>
-        <v>1.0755800000000004</v>
-      </c>
-      <c r="O12">
-        <f t="shared" si="10"/>
-        <v>1.0775600000000001</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="10"/>
-        <v>1.0504499999999997</v>
-      </c>
-      <c r="Q12">
-        <f t="shared" si="10"/>
-        <v>1.12819</v>
-      </c>
-      <c r="R12">
-        <f t="shared" si="10"/>
-        <v>1.0814899999999987</v>
-      </c>
-      <c r="S12">
-        <f>AVERAGE(M12:R12)</f>
-        <v>1.0843266666666664</v>
-      </c>
-      <c r="T12" s="4">
-        <v>1.7044207600000001</v>
-      </c>
-      <c r="U12">
-        <v>62</v>
-      </c>
-      <c r="V12">
-        <v>1.5538847117700001E-2</v>
-      </c>
-      <c r="X12">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="G13">
-        <v>-8.7072599999999998</v>
-      </c>
-      <c r="H13">
-        <v>8.6921499999999998</v>
-      </c>
-      <c r="I13">
-        <v>-8.6939299999999999</v>
-      </c>
-      <c r="J13">
-        <v>8.6645500000000002</v>
-      </c>
-      <c r="K13">
-        <v>-8.7439300000000006</v>
-      </c>
-      <c r="L13">
-        <v>8.6996699999999993</v>
-      </c>
-      <c r="M13">
-        <f>ABS(G13)-$F$2</f>
-        <v>1.1060599999999994</v>
-      </c>
-      <c r="N13">
-        <f t="shared" si="10"/>
-        <v>1.0909499999999994</v>
-      </c>
-      <c r="O13">
-        <f t="shared" si="10"/>
-        <v>1.0927299999999995</v>
-      </c>
-      <c r="P13">
-        <f t="shared" si="10"/>
-        <v>1.0633499999999998</v>
-      </c>
-      <c r="Q13">
-        <f t="shared" si="10"/>
-        <v>1.1427300000000002</v>
-      </c>
-      <c r="R13">
-        <f t="shared" si="10"/>
-        <v>1.0984699999999989</v>
-      </c>
-      <c r="S13">
-        <f>AVERAGE(M13:R13)</f>
-        <v>1.099048333333333</v>
-      </c>
-      <c r="T13" s="4">
-        <v>1.7044207600000001</v>
-      </c>
-      <c r="U13">
-        <v>95</v>
-      </c>
-      <c r="V13">
-        <v>1.5689999999999999E-2</v>
-      </c>
-      <c r="X13">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
-      <c r="G14">
-        <v>-8.6917600000000004</v>
-      </c>
-      <c r="H14">
-        <v>8.6745800000000006</v>
-      </c>
-      <c r="I14">
-        <v>-8.6766000000000005</v>
-      </c>
-      <c r="J14">
-        <v>8.6495800000000003</v>
-      </c>
-      <c r="K14">
-        <v>-8.7271599999999996</v>
-      </c>
-      <c r="L14">
-        <v>8.6804900000000007</v>
-      </c>
-      <c r="M14">
-        <f>ABS(G14)-$F$2</f>
-        <v>1.09056</v>
-      </c>
-      <c r="N14">
-        <f t="shared" si="10"/>
-        <v>1.0733800000000002</v>
-      </c>
-      <c r="O14">
-        <f t="shared" si="10"/>
-        <v>1.0754000000000001</v>
-      </c>
-      <c r="P14">
-        <f t="shared" si="10"/>
-        <v>1.0483799999999999</v>
-      </c>
-      <c r="Q14">
-        <f t="shared" si="10"/>
-        <v>1.1259599999999992</v>
-      </c>
-      <c r="R14">
-        <f t="shared" si="10"/>
-        <v>1.0792900000000003</v>
-      </c>
-      <c r="S14">
-        <f>AVERAGE(M14:R14)</f>
-        <v>1.0821616666666667</v>
-      </c>
-      <c r="T14" s="4">
-        <v>1.7044207600000001</v>
-      </c>
-      <c r="V14">
-        <v>1.55155E-2</v>
-      </c>
-      <c r="W14">
+      <c r="L19" s="9">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M19" s="9">
+        <f>-8.79285</f>
+        <v>-8.7928499999999996</v>
+      </c>
+      <c r="N19" s="9">
+        <v>8.7698599999999995</v>
+      </c>
+      <c r="O19" s="9">
+        <v>-8.7635299999999994</v>
+      </c>
+      <c r="P19" s="9">
+        <v>8.7483000000000004</v>
+      </c>
+      <c r="Q19" s="9">
+        <v>-8.7900700000000001</v>
+      </c>
+      <c r="R19" s="9">
+        <v>8.7693300000000001</v>
+      </c>
+      <c r="S19" s="9" cm="1">
+        <f t="array" ref="S19">AVERAGE(ABS(M19:R19))</f>
+        <v>8.7723233333333326</v>
+      </c>
+      <c r="T19" s="9">
+        <f t="shared" si="0"/>
+        <v>0.37859565534093659</v>
+      </c>
+      <c r="U19" s="9">
+        <v>106</v>
+      </c>
+      <c r="V19" s="9">
+        <v>1.06106E-2</v>
+      </c>
+      <c r="W19" s="9">
         <v>0.1</v>
       </c>
-      <c r="X14">
+      <c r="X19" s="9">
         <v>1000</v>
       </c>
     </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="L20" s="9">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M20" s="11">
+        <v>-8.8119200000000006</v>
+      </c>
+      <c r="N20">
+        <v>8.7890599999999992</v>
+      </c>
+      <c r="O20">
+        <v>-8.7820199999999993</v>
+      </c>
+      <c r="P20">
+        <v>8.7668499999999998</v>
+      </c>
+      <c r="Q20">
+        <v>-8.8094900000000003</v>
+      </c>
+      <c r="R20">
+        <v>8.7887599999999999</v>
+      </c>
+      <c r="S20" s="9" cm="1">
+        <f t="array" ref="S20">AVERAGE(ABS(M20:R20))</f>
+        <v>8.7913499999999996</v>
+      </c>
+      <c r="T20" s="9">
+        <f t="shared" si="0"/>
+        <v>0.16252253750126017</v>
+      </c>
+      <c r="U20">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="L21" s="10">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M21" s="10">
+        <v>-8.8310499999999994</v>
+      </c>
+      <c r="N21" s="10">
+        <v>8.8083299999999998</v>
+      </c>
+      <c r="O21" s="10">
+        <v>-8.8005700000000004</v>
+      </c>
+      <c r="P21" s="10">
+        <v>8.7854899999999994</v>
+      </c>
+      <c r="Q21" s="10">
+        <v>-8.8290100000000002</v>
+      </c>
+      <c r="R21" s="10">
+        <v>8.8082899999999995</v>
+      </c>
+      <c r="S21" s="10" cm="1">
+        <f t="array" ref="S21">AVERAGE(ABS(M21:R21))</f>
+        <v>8.810456666666667</v>
+      </c>
+      <c r="T21" s="10">
+        <f>ABS(L21-S21)/L21*100</f>
+        <v>5.4459086790446101E-2</v>
+      </c>
+      <c r="U21" s="10">
+        <v>108</v>
+      </c>
+      <c r="V21" s="10">
+        <v>1.0810800000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="L22">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="M22">
+        <v>-8.8502200000000002</v>
+      </c>
+      <c r="N22">
+        <v>8.8276699999999995</v>
+      </c>
+      <c r="O22">
+        <v>-8.8191500000000005</v>
+      </c>
+      <c r="P22">
+        <v>8.8042099999999994</v>
+      </c>
+      <c r="Q22">
+        <v>-8.8486100000000008</v>
+      </c>
+      <c r="R22">
+        <v>8.8279099999999993</v>
+      </c>
+      <c r="S22" cm="1">
+        <f t="array" ref="S22">AVERAGE(ABS(M22:R22))</f>
+        <v>8.8296283333333321</v>
+      </c>
+      <c r="T22">
+        <f>ABS(L22-S22)/L22*100</f>
+        <v>0.27217887257439383</v>
+      </c>
+      <c r="U22">
+        <v>109</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
-    <mergeCell ref="M1:R1"/>
+  <mergeCells count="3">
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="O1:P1"/>
+    <mergeCell ref="Q1:R1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FE42C75-AF31-BC43-A94E-9E5F221C005D}">
+  <dimension ref="A1:W12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J22" sqref="J22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="4.83203125" customWidth="1"/>
+    <col min="3" max="4" width="5.83203125" customWidth="1"/>
+    <col min="5" max="5" width="4.1640625" customWidth="1"/>
+    <col min="6" max="6" width="3.6640625" customWidth="1"/>
+    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="8" max="8" width="4" customWidth="1"/>
+    <col min="9" max="9" width="7.83203125" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" customWidth="1"/>
+    <col min="11" max="11" width="6.5" customWidth="1"/>
+    <col min="12" max="12" width="8.33203125" customWidth="1"/>
+    <col min="13" max="13" width="7.83203125" customWidth="1"/>
+    <col min="14" max="14" width="8.5" customWidth="1"/>
+    <col min="15" max="15" width="7.33203125" customWidth="1"/>
+    <col min="16" max="16" width="6.6640625" customWidth="1"/>
+    <col min="17" max="17" width="7.5" customWidth="1"/>
+    <col min="18" max="18" width="8.33203125" customWidth="1"/>
+    <col min="19" max="19" width="7.33203125" customWidth="1"/>
+    <col min="20" max="20" width="7.6640625" customWidth="1"/>
+    <col min="21" max="21" width="6" customWidth="1"/>
+    <col min="22" max="22" width="5.5" customWidth="1"/>
+    <col min="23" max="23" width="8.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" t="s">
+        <v>36</v>
+      </c>
+      <c r="H1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="T1" t="s">
+        <v>44</v>
+      </c>
+      <c r="U1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V1" t="s">
+        <v>65</v>
+      </c>
+      <c r="W1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2">
+        <v>0.8</v>
+      </c>
+      <c r="C2">
+        <v>0.8</v>
+      </c>
+      <c r="D2">
+        <v>0.8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>66</v>
+      </c>
+      <c r="G2">
+        <v>0.1</v>
+      </c>
+      <c r="H2">
+        <v>0.5</v>
+      </c>
+      <c r="I2">
+        <v>7.1012000000000004</v>
+      </c>
+      <c r="J2">
+        <f>I2+H2</f>
+        <v>7.6012000000000004</v>
+      </c>
+      <c r="K2">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="L2">
+        <v>-8.4408700000000003</v>
+      </c>
+      <c r="M2">
+        <v>8.2546499999999998</v>
+      </c>
+      <c r="N2">
+        <v>-8.4459499999999998</v>
+      </c>
+      <c r="O2">
+        <v>8.2396799999999999</v>
+      </c>
+      <c r="P2">
+        <v>-8.4464400000000008</v>
+      </c>
+      <c r="Q2">
+        <v>8.2426999999999992</v>
+      </c>
+      <c r="R2" cm="1">
+        <f t="array" ref="R2">AVERAGE((ABS(L2:Q2)))</f>
+        <v>8.3450483333333345</v>
+      </c>
+      <c r="S2">
+        <f>(K2-R2)/K2*100</f>
+        <v>5.2308718339470612</v>
+      </c>
+      <c r="T2">
+        <v>0.1</v>
+      </c>
+      <c r="U2">
+        <v>99</v>
+      </c>
+      <c r="V2">
+        <v>100</v>
+      </c>
+      <c r="W2">
+        <f>T2/U2*V2</f>
+        <v>0.10101010101010101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="L4">
+        <v>-8.8784100000000006</v>
+      </c>
+      <c r="M4">
+        <v>8.6390200000000004</v>
+      </c>
+      <c r="N4">
+        <v>-8.88523</v>
+      </c>
+      <c r="O4">
+        <v>8.6186600000000002</v>
+      </c>
+      <c r="P4">
+        <v>-8.8884299999999996</v>
+      </c>
+      <c r="Q4">
+        <v>8.6188199999999995</v>
+      </c>
+      <c r="R4" cm="1">
+        <f t="array" ref="R4">AVERAGE((ABS(L4:Q4)))</f>
+        <v>8.754761666666667</v>
+      </c>
+      <c r="S4">
+        <f>(K4-R4)/K4*100</f>
+        <v>0.57803174877791064</v>
+      </c>
+      <c r="T4">
+        <v>0.2</v>
+      </c>
+      <c r="U4">
+        <v>99</v>
+      </c>
+      <c r="V4">
+        <v>64</v>
+      </c>
+      <c r="W4">
+        <f>T4/U4*V4</f>
+        <v>0.12929292929292929</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="L5">
+        <v>-8.9122699999999995</v>
+      </c>
+      <c r="M5">
+        <v>8.6691400000000005</v>
+      </c>
+      <c r="N5">
+        <v>-8.9196000000000009</v>
+      </c>
+      <c r="O5">
+        <v>8.6487099999999995</v>
+      </c>
+      <c r="P5">
+        <v>-8.9228900000000007</v>
+      </c>
+      <c r="Q5">
+        <v>8.6482700000000001</v>
+      </c>
+      <c r="R5" cm="1">
+        <f t="array" ref="R5">AVERAGE((ABS(L5:Q5)))</f>
+        <v>8.7868133333333347</v>
+      </c>
+      <c r="S5">
+        <f>(K5-R5)/K5*100</f>
+        <v>0.21404242421809225</v>
+      </c>
+      <c r="T5">
+        <v>0.2</v>
+      </c>
+      <c r="U5">
+        <v>99</v>
+      </c>
+      <c r="V5">
+        <v>65</v>
+      </c>
+      <c r="W5">
+        <f>T5/U5*V5</f>
+        <v>0.13131313131313133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>8.8056611839999999</v>
+      </c>
+      <c r="L6">
+        <v>-8.9464600000000001</v>
+      </c>
+      <c r="M6">
+        <v>8.6995900000000006</v>
+      </c>
+      <c r="N6">
+        <v>-8.9544200000000007</v>
+      </c>
+      <c r="O6">
+        <v>8.6791599999999995</v>
+      </c>
+      <c r="P6">
+        <v>-8.9577799999999996</v>
+      </c>
+      <c r="Q6">
+        <v>8.6780399999999993</v>
+      </c>
+      <c r="R6" cm="1">
+        <f t="array" ref="R6">AVERAGE((ABS(L6:Q6)))</f>
+        <v>8.8192416666666649</v>
+      </c>
+      <c r="S6">
+        <f>(K6-R6)/K6*100</f>
+        <v>-0.15422445155329073</v>
+      </c>
+      <c r="T6">
+        <v>0.2</v>
+      </c>
+      <c r="U6">
+        <v>99</v>
+      </c>
+      <c r="V6">
+        <v>66</v>
+      </c>
+      <c r="W6" s="6">
+        <f>T6/U6*V6</f>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="G8" s="10">
+        <v>2.8620689655172414E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10">
+        <v>0.8</v>
+      </c>
+      <c r="C10">
+        <v>0.8</v>
+      </c>
+      <c r="D10">
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="10">
+        <v>4.4999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="G12">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="L1:M1"/>
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3165722-1A40-C040-B71B-E1C73DAF83C1}">
+  <dimension ref="A1:R9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" customWidth="1"/>
+    <col min="2" max="2" width="8.83203125" customWidth="1"/>
+    <col min="3" max="3" width="6.83203125" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.33203125" customWidth="1"/>
+    <col min="7" max="7" width="5.33203125" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" customWidth="1"/>
+    <col min="9" max="9" width="7.5" customWidth="1"/>
+    <col min="10" max="10" width="6.33203125" customWidth="1"/>
+    <col min="11" max="11" width="7.6640625" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" customWidth="1"/>
+    <col min="16" max="16" width="9.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+      <c r="G1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" t="s">
+        <v>58</v>
+      </c>
+      <c r="N1" t="s">
+        <v>30</v>
+      </c>
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+      <c r="P1" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>60</v>
+      </c>
+      <c r="R1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1.1E-4</v>
+      </c>
+      <c r="B2" s="10">
+        <v>2.3599999999999999E-2</v>
+      </c>
+      <c r="C2">
+        <v>0.49</v>
+      </c>
+      <c r="D2">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="E2">
+        <f>A2/(2*(1+C2))</f>
+        <v>3.6912751677852349E-5</v>
+      </c>
+      <c r="F2">
+        <f>B2/(2*(1+D2))</f>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="G2">
+        <v>0.5</v>
+      </c>
+      <c r="H2">
+        <v>7.1012000000000004</v>
+      </c>
+      <c r="I2">
+        <f>H2+G2</f>
+        <v>7.6012000000000004</v>
+      </c>
+      <c r="J2">
+        <v>0.4</v>
+      </c>
+      <c r="K2">
+        <v>0.4</v>
+      </c>
+      <c r="L2">
+        <v>0.4</v>
+      </c>
+      <c r="M2">
+        <v>1.06E-2</v>
+      </c>
+      <c r="N2">
+        <v>1000</v>
+      </c>
+      <c r="O2">
+        <v>6</v>
+      </c>
+      <c r="P2">
+        <f>M2/N2*O2</f>
+        <v>6.3600000000000001E-5</v>
+      </c>
+      <c r="Q2">
+        <v>8414</v>
+      </c>
+      <c r="R2">
+        <v>25380</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>0.4</v>
+      </c>
+      <c r="K3">
+        <v>0.8</v>
+      </c>
+      <c r="L3">
+        <v>1.2</v>
+      </c>
+      <c r="M3">
+        <v>1.06E-2</v>
+      </c>
+      <c r="N3">
+        <v>1000</v>
+      </c>
+      <c r="O3">
+        <v>4</v>
+      </c>
+      <c r="P3">
+        <f>M3/N3*O3</f>
+        <v>4.2400000000000001E-5</v>
+      </c>
+      <c r="Q3">
+        <v>2552</v>
+      </c>
+      <c r="R3">
+        <v>7694</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>0.2</v>
+      </c>
+      <c r="K4">
+        <v>0.5</v>
+      </c>
+      <c r="L4">
+        <v>1.2</v>
+      </c>
+      <c r="M4">
+        <v>1.06E-2</v>
+      </c>
+      <c r="N4">
+        <v>2000</v>
+      </c>
+      <c r="O4">
+        <v>8</v>
+      </c>
+      <c r="P4">
+        <f>M4/N4*O4</f>
+        <v>4.2400000000000001E-5</v>
+      </c>
+      <c r="Q4">
+        <v>6476</v>
+      </c>
+      <c r="R4">
+        <v>19538</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="M5">
+        <v>1.06E-2</v>
+      </c>
+      <c r="N5">
+        <v>1000</v>
+      </c>
+      <c r="O5">
+        <v>5</v>
+      </c>
+      <c r="P5">
+        <f>M5/N5*O5</f>
+        <v>5.3000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="J6">
+        <v>0.1</v>
+      </c>
+      <c r="K6">
+        <v>0.5</v>
+      </c>
+      <c r="L6">
+        <v>1.2</v>
+      </c>
+      <c r="M6">
+        <v>1.06E-2</v>
+      </c>
+      <c r="N6">
+        <v>1000</v>
+      </c>
+      <c r="P6">
+        <f>M6/N6*O6</f>
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>9292</v>
+      </c>
+      <c r="R6">
+        <v>29986</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1.1E-4</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0.13274</v>
+      </c>
+      <c r="C8">
+        <v>0.49</v>
+      </c>
+      <c r="D8">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="E8">
+        <f>A8/(2*(1+C8))</f>
+        <v>3.6912751677852349E-5</v>
+      </c>
+      <c r="F8">
+        <f>B8/(2*(1+D8))</f>
+        <v>4.4996610169491524E-2</v>
+      </c>
+      <c r="G8">
+        <v>0.5</v>
+      </c>
+      <c r="H8">
+        <v>7.1012000000000004</v>
+      </c>
+      <c r="I8">
+        <f>H8+G8</f>
+        <v>7.6012000000000004</v>
+      </c>
+      <c r="J8">
+        <v>0.1</v>
+      </c>
+      <c r="K8">
+        <v>0.5</v>
+      </c>
+      <c r="L8">
+        <v>1.2</v>
+      </c>
+      <c r="M8">
+        <v>1.06E-2</v>
+      </c>
+      <c r="N8">
+        <v>1000</v>
+      </c>
+      <c r="O8">
+        <v>5</v>
+      </c>
+      <c r="P8">
+        <f>M8/N8*O8</f>
+        <v>5.3000000000000001E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1.1E-4</v>
+      </c>
+      <c r="B9" s="10">
+        <v>0.29499999999999998</v>
+      </c>
+      <c r="C9">
+        <v>0.49</v>
+      </c>
+      <c r="D9">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="E9">
+        <f>A9/(2*(1+C9))</f>
+        <v>3.6912751677852349E-5</v>
+      </c>
+      <c r="F9">
+        <f>B9/(2*(1+D9))</f>
+        <v>9.9999999999999992E-2</v>
+      </c>
+      <c r="G9">
+        <v>0.5</v>
+      </c>
+      <c r="H9">
+        <v>7.1012000000000004</v>
+      </c>
+      <c r="I9">
+        <f>H9+G9</f>
+        <v>7.6012000000000004</v>
+      </c>
+      <c r="J9">
+        <v>0.1</v>
+      </c>
+      <c r="K9">
+        <v>0.5</v>
+      </c>
+      <c r="L9">
+        <v>1.2</v>
+      </c>
+      <c r="M9">
+        <v>1.06E-2</v>
+      </c>
+      <c r="N9">
+        <v>1000</v>
+      </c>
+      <c r="P9">
+        <f>M9/N9*O9</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>